<commit_message>
updated excel sheets for bitbucket
</commit_message>
<xml_diff>
--- a/bitbucket-ado/bitbucket-to-azure.xlsx
+++ b/bitbucket-ado/bitbucket-to-azure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsharma\Desktop\version control excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abharamagoudar\Desktop\api\github\SCM-Migration-DEMO\bitbucket-ado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254CF341-B760-4027-8998-F79FE1F5DA1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1A5899-CFE9-43E3-8F1F-130CA95B2594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>sr</t>
   </si>
@@ -39,16 +39,25 @@
     <t>workspace_id</t>
   </si>
   <si>
-    <t>varun160799</t>
-  </si>
-  <si>
-    <t>devops-TEKsystems/test</t>
-  </si>
-  <si>
-    <t>you-dont-need-javascript</t>
-  </si>
-  <si>
-    <t>python-private</t>
+    <t>anilgoudasb06</t>
+  </si>
+  <si>
+    <t>almatasks</t>
+  </si>
+  <si>
+    <t>app-n-pak</t>
+  </si>
+  <si>
+    <t>casa-build-utils</t>
+  </si>
+  <si>
+    <t>casaplotserver</t>
+  </si>
+  <si>
+    <t>casashell</t>
+  </si>
+  <si>
+    <t>anilbharamagoudar06/Anil-devops</t>
   </si>
 </sst>
 </file>
@@ -375,20 +384,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,7 +411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -410,13 +419,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -424,10 +433,52 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated excel sheet for bitbucket-ado
</commit_message>
<xml_diff>
--- a/bitbucket-ado/bitbucket-to-azure.xlsx
+++ b/bitbucket-ado/bitbucket-to-azure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abharamagoudar\Desktop\api\github\SCM-Migration-DEMO\bitbucket-ado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B28A38B-F691-4E57-9635-CF5EF883A962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C625E2-984B-47EA-A331-C1E36D218490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>sr</t>
   </si>
@@ -42,9 +42,6 @@
     <t>anilgoudasb06</t>
   </si>
   <si>
-    <t>almatasks</t>
-  </si>
-  <si>
     <t>app-n-pak</t>
   </si>
   <si>
@@ -57,19 +54,7 @@
     <t>casashell</t>
   </si>
   <si>
-    <t>casatablebrowser</t>
-  </si>
-  <si>
-    <t>casatestdata-large</t>
-  </si>
-  <si>
     <t>casafeather</t>
-  </si>
-  <si>
-    <t>casampi</t>
-  </si>
-  <si>
-    <t>casa-asap</t>
   </si>
   <si>
     <t>repo-migartion/git-project</t>
@@ -399,16 +384,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -437,7 +422,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -451,7 +436,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -465,7 +450,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -479,7 +464,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -493,77 +478,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>